<commit_message>
added some test cases in used cars feature
</commit_message>
<xml_diff>
--- a/Excel/Hackathon_Functional.xlsx
+++ b/Excel/Hackathon_Functional.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2317992_cognizant_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2318507\eclipse-workspace\IdentifyNewBikes_Hackathon\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{01D8ACD4-8FAB-47F6-B774-F8D7A796C892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C08C769F-D118-436E-BBC4-862F4FC19FC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5872D2-5D10-4E2D-A81C-83D4A4FC03BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{DEE1165F-28CB-4AE3-8939-EFF4B6CA8DEB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="107">
   <si>
     <t>MODULE</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>TC_002</t>
-  </si>
-  <si>
-    <t>Validate the click function on Upcoming bikes</t>
   </si>
   <si>
     <t xml:space="preserve">1.Open the website(Zigwheels.com)
@@ -123,9 +120,6 @@
   </si>
   <si>
     <t>TC_003</t>
-  </si>
-  <si>
-    <t>Validate the manufacturers dropdown</t>
   </si>
   <si>
     <t xml:space="preserve">1.Open the website(Zigwheels.com)
@@ -142,20 +136,11 @@
     <t>TC_004</t>
   </si>
   <si>
-    <t>Validate the Honda button in the drop down</t>
-  </si>
-  <si>
     <t>On selecting Honda brand only Honda 
 bikes are displayed</t>
   </si>
   <si>
-    <t>Validate the hover function over New bikes</t>
-  </si>
-  <si>
     <t>TC_005</t>
-  </si>
-  <si>
-    <t>Validate the Viewmore button</t>
   </si>
   <si>
     <t xml:space="preserve">1.Open the website(Zigwheels.com)
@@ -375,6 +360,57 @@
   </si>
   <si>
     <t>TC_013</t>
+  </si>
+  <si>
+    <t>Validate whether a drop down menu is occurred
+when the mouse is hovered over the 'NewBikes' (upcoming Bikes).</t>
+  </si>
+  <si>
+    <t>Validate the upcoming bikes option is clickable 
+and redirecting to an appropriate page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the drop down menu is visible 
+of the manufacturers after clicking </t>
+  </si>
+  <si>
+    <t>Validate that all the honda bikes are being displayed
+after selecting the honda option in the drop down 
+of manufacturers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate whether 'view more' option is visible </t>
+  </si>
+  <si>
+    <t>Validate that 'view more' option is working or not if
+the number of rows of bikes is more than 3</t>
+  </si>
+  <si>
+    <t>Validate whether the names of the bikes are 
+being displayed or not</t>
+  </si>
+  <si>
+    <t>Validate whether the price of the bikes are being 
+displayed or not</t>
+  </si>
+  <si>
+    <t>Validate whether the expected dates of the bikes
+are displayed or not</t>
+  </si>
+  <si>
+    <t>TC_014</t>
+  </si>
+  <si>
+    <t>TC_015</t>
+  </si>
+  <si>
+    <t>TC_016</t>
+  </si>
+  <si>
+    <t>TC_017</t>
+  </si>
+  <si>
+    <t>Test case id</t>
   </si>
 </sst>
 </file>
@@ -802,7 +838,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -816,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -830,7 +866,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -841,10 +877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10AE18E0-BAEA-4F7B-947B-A477766B61F1}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>106</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>15</v>
@@ -898,8 +934,8 @@
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
+      <c r="C2" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -908,373 +944,421 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
+      <c r="C3" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" t="s">
-        <v>77</v>
-      </c>
+      <c r="C10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>67</v>
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" t="s">
-        <v>76</v>
+        <v>51</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1306,34 +1390,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>16</v>
@@ -1341,37 +1425,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I2" s="3">
         <v>45369</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1398,19 +1482,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1418,16 +1502,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1435,16 +1519,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1452,16 +1536,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>